<commit_message>
acqua dati CSV sistemato
</commit_message>
<xml_diff>
--- a/08_VENTURI/venturi_dati.xlsx
+++ b/08_VENTURI/venturi_dati.xlsx
@@ -93,8 +93,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="160" formatCode="0.000"/>
+    <numFmt numFmtId="161" formatCode="0.000000"/>
+    <numFmt numFmtId="162" formatCode="0.0000000"/>
   </numFmts>
   <fonts count="1">
     <font>
@@ -124,7 +126,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="2" xfId="0" applyNumberFormat="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="1" xfId="0" applyNumberFormat="1"/>
@@ -136,7 +138,8 @@
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="2" xfId="0" applyNumberFormat="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="161" xfId="0" applyNumberFormat="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="162" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1455,6 +1458,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
+    <col bestFit="1" min="5" max="5" width="9.6640625"/>
     <col bestFit="1" min="10" max="10" width="10.5234375"/>
   </cols>
   <sheetData>
@@ -1501,15 +1505,15 @@
         <v>0.32500000000000001</v>
       </c>
       <c r="C2" s="3">
-        <f>B2-$J$2</f>
+        <f t="shared" ref="C2:C6" si="0">B2-$J$2</f>
         <v>0.23600000000000002</v>
       </c>
-      <c r="D2">
-        <f>C2/1000</f>
+      <c r="D2" s="7">
+        <f t="shared" ref="D2:D6" si="1">C2/1000</f>
         <v>0.00023600000000000002</v>
       </c>
-      <c r="E2">
-        <f>D2/$K$2</f>
+      <c r="E2" s="8">
+        <f t="shared" ref="E2:E6" si="2">D2/$K$2</f>
         <v>2.3600000000000001e-05</v>
       </c>
       <c r="F2" s="1">
@@ -1518,7 +1522,7 @@
       <c r="G2" s="1">
         <v>101.53</v>
       </c>
-      <c r="H2" s="7">
+      <c r="H2" s="1">
         <v>101.58</v>
       </c>
       <c r="I2" s="1">
@@ -1539,15 +1543,15 @@
         <v>0.41499999999999998</v>
       </c>
       <c r="C3" s="3">
-        <f>B3-$J$2</f>
+        <f t="shared" si="0"/>
         <v>0.32599999999999996</v>
       </c>
-      <c r="D3">
-        <f>C3/1000</f>
+      <c r="D3" s="7">
+        <f t="shared" si="1"/>
         <v>0.00032599999999999996</v>
       </c>
-      <c r="E3">
-        <f>D3/$K$2</f>
+      <c r="E3" s="8">
+        <f t="shared" si="2"/>
         <v>3.2599999999999993e-05</v>
       </c>
       <c r="F3" s="1">
@@ -1571,15 +1575,15 @@
         <v>0.503</v>
       </c>
       <c r="C4" s="3">
-        <f>B4-$J$2</f>
+        <f t="shared" si="0"/>
         <v>0.41400000000000003</v>
       </c>
-      <c r="D4">
-        <f>C4/1000</f>
+      <c r="D4" s="7">
+        <f t="shared" si="1"/>
         <v>0.00041400000000000003</v>
       </c>
-      <c r="E4">
-        <f>D4/$K$2</f>
+      <c r="E4" s="8">
+        <f t="shared" si="2"/>
         <v>4.1400000000000003e-05</v>
       </c>
       <c r="F4" s="1">
@@ -1603,15 +1607,15 @@
         <v>0.55700000000000005</v>
       </c>
       <c r="C5" s="3">
-        <f>B5-$J$2</f>
+        <f t="shared" si="0"/>
         <v>0.46800000000000008</v>
       </c>
-      <c r="D5">
-        <f>C5/1000</f>
+      <c r="D5" s="7">
+        <f t="shared" si="1"/>
         <v>0.0004680000000000001</v>
       </c>
-      <c r="E5">
-        <f>D5/$K$2</f>
+      <c r="E5" s="8">
+        <f t="shared" si="2"/>
         <v>4.6800000000000013e-05</v>
       </c>
       <c r="F5" s="1">
@@ -1635,15 +1639,15 @@
         <v>0.66600000000000004</v>
       </c>
       <c r="C6" s="3">
-        <f>B6-$J$2</f>
+        <f t="shared" si="0"/>
         <v>0.57700000000000007</v>
       </c>
-      <c r="D6">
-        <f>C6/1000</f>
+      <c r="D6" s="7">
+        <f t="shared" si="1"/>
         <v>0.00057700000000000004</v>
       </c>
-      <c r="E6">
-        <f>D6/$K$2</f>
+      <c r="E6" s="8">
+        <f t="shared" si="2"/>
         <v>5.7700000000000007e-05</v>
       </c>
       <c r="F6" s="1">

</xml_diff>